<commit_message>
Put out the fire
</commit_message>
<xml_diff>
--- a/DnData/D20/NJT/MYLUCK_22Camp_Blixt.xlsx
+++ b/DnData/D20/NJT/MYLUCK_22Camp_Blixt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\DnData\D20\NJT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB23B851-D2CE-40C0-BBC4-A5CE0D406707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AA88BD-2190-4998-8B7C-C45CC78BEE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{555EC10F-2DA9-4A2E-ABDF-A872F8AFBE1A}"/>
   </bookViews>
@@ -315,7 +315,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5</c:v>
@@ -969,7 +969,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5</c:v>
@@ -2706,7 +2706,7 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="C2" s="3">
         <f>B2/B22 * 100</f>
-        <v>4.918032786885246</v>
+        <v>4.838709677419355</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1">
@@ -2766,11 +2766,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3">
         <f>B3/B22 * 100</f>
-        <v>8.1967213114754092</v>
+        <v>9.67741935483871</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="C4" s="3">
         <f>B4/B22 * 100</f>
-        <v>8.1967213114754092</v>
+        <v>8.064516129032258</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1">
@@ -2812,7 +2812,7 @@
       </c>
       <c r="C5" s="3">
         <f>B5/B22 * 100</f>
-        <v>3.278688524590164</v>
+        <v>3.225806451612903</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="C6" s="3">
         <f>B6/B22 * 100</f>
-        <v>4.918032786885246</v>
+        <v>4.838709677419355</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1">
@@ -2873,7 +2873,7 @@
       </c>
       <c r="C8" s="3">
         <f>B8/B22 * 100</f>
-        <v>6.557377049180328</v>
+        <v>6.4516129032258061</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1">
@@ -2894,7 +2894,7 @@
       </c>
       <c r="C9" s="3">
         <f>B9/B22 * 100</f>
-        <v>4.918032786885246</v>
+        <v>4.838709677419355</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1">
@@ -2915,7 +2915,7 @@
       </c>
       <c r="C10" s="3">
         <f>B10/B22 * 100</f>
-        <v>1.639344262295082</v>
+        <v>1.6129032258064515</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1">
@@ -2936,7 +2936,7 @@
       </c>
       <c r="C11" s="3">
         <f>B11/B22 * 100</f>
-        <v>4.918032786885246</v>
+        <v>4.838709677419355</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1">
@@ -2957,7 +2957,7 @@
       </c>
       <c r="C12" s="3">
         <f>B12/B22 * 100</f>
-        <v>6.557377049180328</v>
+        <v>6.4516129032258061</v>
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="1">
@@ -2978,7 +2978,7 @@
       </c>
       <c r="C13" s="3">
         <f>B13/B22 * 100</f>
-        <v>3.278688524590164</v>
+        <v>3.225806451612903</v>
       </c>
       <c r="Q13" s="1"/>
       <c r="R13" s="1">
@@ -2999,7 +2999,7 @@
       </c>
       <c r="C14" s="3">
         <f>B14/B22 * 100</f>
-        <v>8.1967213114754092</v>
+        <v>8.064516129032258</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="C15" s="3">
         <f>B15/B22 * 100</f>
-        <v>3.278688524590164</v>
+        <v>3.225806451612903</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1">
@@ -3041,7 +3041,7 @@
       </c>
       <c r="C16" s="3">
         <f>B16/B22 * 100</f>
-        <v>8.1967213114754092</v>
+        <v>8.064516129032258</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="C17" s="3">
         <f>B17/B22 * 100</f>
-        <v>4.918032786885246</v>
+        <v>4.838709677419355</v>
       </c>
       <c r="Q17" s="1"/>
       <c r="R17" s="1">
@@ -3083,7 +3083,7 @@
       </c>
       <c r="C18" s="3">
         <f>B18/B22 * 100</f>
-        <v>3.278688524590164</v>
+        <v>3.225806451612903</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="1">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="C19" s="3">
         <f>B19/B22 * 100</f>
-        <v>4.918032786885246</v>
+        <v>4.838709677419355</v>
       </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1">
@@ -3128,7 +3128,7 @@
       </c>
       <c r="C20" s="3">
         <f>B20/B22 * 100</f>
-        <v>3.278688524590164</v>
+        <v>3.225806451612903</v>
       </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1">
@@ -3149,7 +3149,7 @@
       </c>
       <c r="C21" s="3">
         <f>B21/B22 * 100</f>
-        <v>6.557377049180328</v>
+        <v>6.4516129032258061</v>
       </c>
       <c r="Q21" s="1"/>
       <c r="R21" s="1">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="B22">
         <f>SUM(B2:B21)</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S22">
         <f>SUM(S2:S21)</f>
@@ -3183,11 +3183,11 @@
       </c>
       <c r="B24">
         <f>SUM(B2:B11)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3">
         <f>SUM(C2:C11)</f>
-        <v>47.540983606557383</v>
+        <v>48.387096774193537</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
@@ -3200,7 +3200,7 @@
       </c>
       <c r="C25" s="3">
         <f>SUM(C12:C21)</f>
-        <v>52.459016393442624</v>
+        <v>51.612903225806448</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">

</xml_diff>